<commit_message>
Añadido esquema base de datos, archivo para importar base de datos y actualizacion de documentos
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/Backlog Priorizado - Proyecto Biblioteca El pimiento.xlsx
+++ b/Fase 2/Evidencias Proyecto/Backlog Priorizado - Proyecto Biblioteca El pimiento.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="111">
   <si>
     <t>Desarrollo ágil: Product Backlog priorizado - Proyecto Biblioteca El pimiento</t>
   </si>
@@ -268,13 +268,19 @@
     <t>E3-H2</t>
   </si>
   <si>
-    <t>Gestionar catálogos</t>
-  </si>
-  <si>
-    <t>Como bibliotecario, quiero poder crear y gestionar diferentes catálogos o colecciones de libros, para organizar mejor los recursos de la biblioteca y facilitar la búsqueda a los usuarios.</t>
+    <t>Filtro categorias</t>
+  </si>
+  <si>
+    <t>Como usuario, quiero ser capaz de ver libros especificos de alguna categoria que yo elija</t>
   </si>
   <si>
     <t>Media</t>
+  </si>
+  <si>
+    <t>Filtro generos</t>
+  </si>
+  <si>
+    <t>Como usuario, quiero ser capaz de ver libros especificos de algun genero que yo elija</t>
   </si>
   <si>
     <t>E5-H1</t>
@@ -529,10 +535,10 @@
         <color rgb="FF284E3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF284E3F"/>
@@ -540,13 +546,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF284E3F"/>
@@ -554,13 +560,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
         <color rgb="FF284E3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF284E3F"/>
@@ -634,13 +640,13 @@
     <xf borderId="8" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -716,7 +722,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B4:F38" displayName="Tabla_1" name="Tabla_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B4:F39" displayName="Tabla_1" name="Tabla_1" id="1">
   <tableColumns count="5">
     <tableColumn name="ID de la Historia" id="1"/>
     <tableColumn name="Nombre de Tarea" id="2"/>
@@ -1426,30 +1432,30 @@
     </row>
     <row r="32">
       <c r="B32" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="D32" s="12" t="s">
         <v>89</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>90</v>
       </c>
       <c r="E32" s="14">
         <v>3.0</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>93</v>
       </c>
       <c r="E33" s="9">
         <v>3.0</v>
@@ -1460,13 +1466,13 @@
     </row>
     <row r="34">
       <c r="B34" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="D34" s="12" t="s">
         <v>95</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>96</v>
       </c>
       <c r="E34" s="14">
         <v>3.0</v>
@@ -1477,69 +1483,86 @@
     </row>
     <row r="35">
       <c r="B35" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="D35" s="7" t="s">
         <v>98</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>99</v>
       </c>
       <c r="E35" s="9">
         <v>3.0</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36">
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="D36" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="E36" s="14">
+        <v>3.0</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="E36" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="B37" s="22" t="s">
+      <c r="C37" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="D37" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>105</v>
       </c>
       <c r="E37" s="9">
         <v>4.0</v>
       </c>
-      <c r="F37" s="23" t="s">
+      <c r="F37" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="38">
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="25" t="s">
+      <c r="D38" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D38" s="26" t="s">
+      <c r="E38" s="14">
+        <v>4.0</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="E38" s="27">
+      <c r="C39" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="E39" s="27">
         <v>4.0</v>
       </c>
-      <c r="F38" s="28" t="s">
+      <c r="F39" s="28" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>